<commit_message>
Updated DB plan, created SQL query
</commit_message>
<xml_diff>
--- a/DB_structure_plan.xlsx
+++ b/DB_structure_plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Farah\Documents\GitHub\Plane-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB389FA-230E-4931-B029-726328E9605F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F90BF646-0034-48BC-A102-ACC15638355C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="18220" windowHeight="11620" xr2:uid="{09BED794-C06F-4425-9A50-D5A9AF03BA90}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="83">
   <si>
     <t>planes</t>
   </si>
@@ -51,9 +51,6 @@
     <t>passport_details</t>
   </si>
   <si>
-    <t>BOOL</t>
-  </si>
-  <si>
     <t>DATE</t>
   </si>
   <si>
@@ -75,6 +72,9 @@
     <t>last_name</t>
   </si>
   <si>
+    <t>role</t>
+  </si>
+  <si>
     <t>plane_id</t>
   </si>
   <si>
@@ -250,6 +250,39 @@
   </si>
   <si>
     <t>FLOAT, litres</t>
+  </si>
+  <si>
+    <t>airline</t>
+  </si>
+  <si>
+    <t>credentials</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>*id</t>
+  </si>
+  <si>
+    <t>VARCHAR(20)</t>
+  </si>
+  <si>
+    <t>VARCHAR(30)30)</t>
+  </si>
+  <si>
+    <t>VARCHAR 30</t>
+  </si>
+  <si>
+    <t>passport_number</t>
+  </si>
+  <si>
+    <t>BIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -387,8 +420,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
@@ -436,6 +472,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -750,396 +792,454 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91E83692-542A-45C2-A9D4-C1011B074B22}">
-  <dimension ref="A6:J31"/>
+  <dimension ref="A6:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="89" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.26953125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.81640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" style="1"/>
-    <col min="5" max="5" width="16.26953125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.90625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.453125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="23.54296875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="22.90625" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="19.26953125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.6328125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19.81640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" style="2"/>
+    <col min="5" max="5" width="16.26953125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="21.90625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="9.453125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="23.54296875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="22.90625" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="E6" s="5" t="s">
+      <c r="C6" s="7"/>
+      <c r="E6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="6"/>
-      <c r="H6" s="5" t="s">
+      <c r="F6" s="7"/>
+      <c r="H6" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="17"/>
-      <c r="J6" s="6"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="18" t="s">
+      <c r="I7" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="J7" s="19"/>
+      <c r="J7" s="20"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="J8" s="20"/>
+    </row>
+    <row r="9" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="C9" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H9" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="I9" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="J9" s="23"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B10" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="24"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="26"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B11" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="H8" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I8" s="18" t="s">
+      <c r="E12" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B15" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="E15" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="7"/>
+      <c r="H15" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="I15" s="7"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B16" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="F18" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="J8" s="19"/>
-    </row>
-    <row r="9" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="8" t="s">
+      <c r="H18" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B19" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="H19" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="I19" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B20" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B21" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B22" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="29" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B23" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="H9" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="I9" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="J9" s="22"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B10" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="8" t="s">
+      <c r="E23" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F23" s="7"/>
+      <c r="H23" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I23" s="7"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E24" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E25" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="H10" s="23"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="25"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B11" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B15" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="13"/>
-      <c r="E15" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F15" s="6"/>
-      <c r="H15" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="I15" s="6"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B16" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="I16" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H17" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="I17" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I18" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B19" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="H19" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="I19" s="15" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B20" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B21" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B22" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="E23" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F23" s="6"/>
-      <c r="H23" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="I23" s="6"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="3"/>
-      <c r="E24" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="H24" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="I24" s="8"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="H25" s="7" t="s">
+      <c r="H25" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I25" s="8" t="s">
+      <c r="I25" s="9" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F26" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="4"/>
+      <c r="E26" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="H26" s="7" t="s">
+      <c r="H26" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="I26" s="8" t="s">
+      <c r="I26" s="9" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H27" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="I27" s="17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="I28" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B29" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E27" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="H27" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="I27" s="16" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="E28" s="14" t="s">
+      <c r="H29" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="I29" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H30" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H31" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="I31" s="12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E33" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F33" s="1"/>
+    </row>
+    <row r="34" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E34" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E35" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E36" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E37" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E38" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F28" s="15" t="s">
+      <c r="F38" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="H28" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="I28" s="8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="H29" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="I29" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="H30" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="I30" s="8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="H31" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="I31" s="11" t="s">
-        <v>71</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
+    <mergeCell ref="E33:F33"/>
     <mergeCell ref="E15:F15"/>
     <mergeCell ref="H15:I15"/>
     <mergeCell ref="H23:I23"/>

</xml_diff>

<commit_message>
documentation for DB, display DB structure.
</commit_message>
<xml_diff>
--- a/DB_structure_plan.xlsx
+++ b/DB_structure_plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Farah\Documents\GitHub\Plane-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A8DF40-23C6-4C78-BABE-8794C93F65AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE2381E-C2A8-4DF4-B0CD-041F10D87C87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="18220" windowHeight="11620" xr2:uid="{09BED794-C06F-4425-9A50-D5A9AF03BA90}"/>
   </bookViews>
@@ -597,12 +597,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -675,9 +669,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -704,6 +695,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1021,35 +1021,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91E83692-542A-45C2-A9D4-C1011B074B22}">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="87" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="O30" sqref="O30"/>
+    <sheetView tabSelected="1" zoomScale="44" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.453125" style="18" customWidth="1"/>
-    <col min="2" max="2" width="19.81640625" style="18" customWidth="1"/>
+    <col min="1" max="1" width="18.453125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="19.81640625" style="16" customWidth="1"/>
     <col min="3" max="3" width="19.54296875" style="7" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" style="18"/>
-    <col min="5" max="5" width="16.26953125" style="18" customWidth="1"/>
-    <col min="6" max="6" width="21.90625" style="18" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" style="16"/>
+    <col min="5" max="5" width="16.26953125" style="16" customWidth="1"/>
+    <col min="6" max="6" width="21.90625" style="16" customWidth="1"/>
     <col min="7" max="7" width="34.36328125" style="7" customWidth="1"/>
-    <col min="8" max="8" width="9.453125" style="18" customWidth="1"/>
-    <col min="9" max="9" width="23.54296875" style="18" customWidth="1"/>
-    <col min="10" max="10" width="22.90625" style="18" customWidth="1"/>
+    <col min="8" max="8" width="9.453125" style="16" customWidth="1"/>
+    <col min="9" max="9" width="23.54296875" style="16" customWidth="1"/>
+    <col min="10" max="10" width="22.90625" style="16" customWidth="1"/>
     <col min="11" max="11" width="34.1796875" style="7" customWidth="1"/>
-    <col min="12" max="16384" width="8.7265625" style="18"/>
+    <col min="12" max="16384" width="8.7265625" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="41" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -1057,738 +1057,738 @@
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="10" t="s">
+      <c r="B4" s="43"/>
+      <c r="C4" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="10" t="s">
+      <c r="F4" s="43"/>
+      <c r="G4" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="42" t="s">
         <v>118</v>
       </c>
-      <c r="J4" s="9"/>
-      <c r="K4" s="10" t="s">
+      <c r="J4" s="43"/>
+      <c r="K4" s="8" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="I5" s="22" t="s">
+      <c r="I5" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="J5" s="16" t="s">
+      <c r="J5" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="K5" s="11" t="s">
+      <c r="K5" s="9" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F6" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="I6" s="22" t="s">
+      <c r="I6" s="20" t="s">
         <v>22</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="K6" s="9" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="F7" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="I7" s="22" t="s">
+      <c r="I7" s="20" t="s">
         <v>51</v>
       </c>
       <c r="J7" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="K7" s="38" t="s">
+      <c r="K7" s="35" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="I8" s="39" t="s">
+      <c r="I8" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="J8" s="19" t="s">
+      <c r="J8" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="K8" s="41" t="s">
+      <c r="K8" s="38" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="E9" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="F9" s="19" t="s">
+      <c r="F9" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="11" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="11" t="s">
         <v>100</v>
       </c>
       <c r="G10" s="6"/>
     </row>
     <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="13" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="10" t="s">
+      <c r="B13" s="43"/>
+      <c r="C13" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="10" t="s">
+      <c r="F13" s="43"/>
+      <c r="G13" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="I13" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="J13" s="9"/>
-      <c r="K13" s="10" t="s">
+      <c r="J13" s="43"/>
+      <c r="K13" s="8" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C14" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="E14" s="22" t="s">
+      <c r="C14" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="16" t="s">
+      <c r="F14" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="G14" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="I14" s="22" t="s">
+      <c r="I14" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="J14" s="16" t="s">
+      <c r="J14" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="K14" s="11" t="s">
+      <c r="K14" s="9" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="E15" s="23" t="s">
+      <c r="E15" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="F15" s="16" t="s">
+      <c r="F15" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="G15" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="I15" s="23" t="s">
+      <c r="I15" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="J15" s="16" t="s">
+      <c r="J15" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="K15" s="11" t="s">
+      <c r="K15" s="9" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="C16" s="11" t="s">
+      <c r="B16" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="E16" s="22" t="s">
+      <c r="E16" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="F16" s="16" t="s">
+      <c r="F16" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="G16" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="I16" s="22" t="s">
+      <c r="I16" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="J16" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="K16" s="11" t="s">
+      <c r="J16" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="K16" s="9" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="E17" s="28" t="s">
+      <c r="E17" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="F17" s="19" t="s">
+      <c r="F17" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="G17" s="13" t="s">
+      <c r="G17" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="I17" s="28" t="s">
+      <c r="I17" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="J17" s="42" t="s">
+      <c r="J17" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="K17" s="36" t="s">
+      <c r="K17" s="33" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="12" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="13" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="21" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="10" t="s">
+      <c r="B21" s="43"/>
+      <c r="C21" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="F21" s="9"/>
-      <c r="G21" s="10" t="s">
+      <c r="F21" s="43"/>
+      <c r="G21" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="I21" s="8" t="s">
+      <c r="I21" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="J21" s="9"/>
-      <c r="K21" s="10" t="s">
+      <c r="J21" s="43"/>
+      <c r="K21" s="8" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C22" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="E22" s="22" t="s">
+      <c r="C22" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="F22" s="16" t="s">
+      <c r="F22" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="G22" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="I22" s="22" t="s">
+      <c r="G22" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="I22" s="20" t="s">
         <v>58</v>
       </c>
       <c r="J22" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="K22" s="11" t="s">
+      <c r="K22" s="9" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A23" s="23" t="s">
+      <c r="A23" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="B23" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="C23" s="11" t="s">
+      <c r="B23" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="E23" s="22" t="s">
+      <c r="E23" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="F23" s="16" t="s">
+      <c r="F23" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="G23" s="11" t="s">
+      <c r="G23" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="I23" s="22" t="s">
+      <c r="I23" s="20" t="s">
         <v>16</v>
       </c>
       <c r="J23" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="K23" s="11" t="s">
+      <c r="K23" s="9" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="E24" s="22" t="s">
+      <c r="E24" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="F24" s="16" t="s">
+      <c r="F24" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="G24" s="11" t="s">
+      <c r="G24" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="I24" s="22" t="s">
+      <c r="I24" s="20" t="s">
         <v>44</v>
       </c>
       <c r="J24" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="K24" s="11" t="s">
+      <c r="K24" s="9" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="20" t="s">
         <v>40</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C25" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="E25" s="22" t="s">
+      <c r="C25" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="F25" s="16" t="s">
+      <c r="F25" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G25" s="12" t="s">
+      <c r="G25" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="I25" s="22" t="s">
+      <c r="I25" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="J25" s="33" t="s">
+      <c r="J25" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="K25" s="43" t="s">
+      <c r="K25" s="40" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="C26" s="14" t="s">
+      <c r="B26" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="E26" s="28" t="s">
+      <c r="E26" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="F26" s="42" t="s">
+      <c r="F26" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="G26" s="36" t="s">
+      <c r="G26" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="I26" s="22" t="s">
+      <c r="I26" s="20" t="s">
         <v>46</v>
       </c>
       <c r="J26" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="K26" s="11" t="s">
+      <c r="K26" s="9" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="25" t="s">
+      <c r="A27" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27" s="15" t="s">
+      <c r="B27" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="I27" s="22" t="s">
+      <c r="I27" s="20" t="s">
         <v>47</v>
       </c>
       <c r="J27" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="K27" s="11" t="s">
+      <c r="K27" s="9" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="I28" s="22" t="s">
+      <c r="I28" s="20" t="s">
         <v>48</v>
       </c>
       <c r="J28" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="K28" s="11" t="s">
+      <c r="K28" s="9" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="I29" s="22" t="s">
+      <c r="I29" s="20" t="s">
         <v>49</v>
       </c>
       <c r="J29" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="K29" s="11" t="s">
+      <c r="K29" s="9" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="29" t="s">
+      <c r="A30" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="I30" s="35" t="s">
+      <c r="B30" s="18"/>
+      <c r="I30" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="J30" s="24" t="s">
+      <c r="J30" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="K30" s="11" t="s">
+      <c r="K30" s="9" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="20" t="s">
+      <c r="A31" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="20" t="s">
+      <c r="B31" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="E31" s="8" t="s">
+      <c r="E31" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="F31" s="9"/>
-      <c r="G31" s="10" t="s">
+      <c r="F31" s="43"/>
+      <c r="G31" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="I31" s="39" t="s">
+      <c r="I31" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="J31" s="40" t="s">
+      <c r="J31" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="K31" s="36" t="s">
+      <c r="K31" s="33" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="20" t="s">
+      <c r="A32" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="20" t="s">
+      <c r="B32" s="18" t="s">
         <v>32</v>
       </c>
       <c r="C32" s="5"/>
-      <c r="E32" s="22" t="s">
+      <c r="E32" s="20" t="s">
         <v>127</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="G32" s="11" t="s">
+      <c r="G32" s="9" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A33" s="30" t="s">
+      <c r="A33" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="20" t="s">
+      <c r="B33" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="E33" s="22" t="s">
+      <c r="E33" s="20" t="s">
         <v>61</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="G33" s="11" t="s">
+      <c r="G33" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="I33" s="8" t="s">
+      <c r="I33" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="J33" s="9"/>
-      <c r="K33" s="10" t="s">
+      <c r="J33" s="43"/>
+      <c r="K33" s="8" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A34" s="21" t="s">
+      <c r="A34" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="B34" s="21" t="s">
+      <c r="B34" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="E34" s="22" t="s">
+      <c r="E34" s="20" t="s">
         <v>62</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="G34" s="11" t="s">
+      <c r="G34" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="I34" s="35" t="s">
+      <c r="I34" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="J34" s="16" t="s">
+      <c r="J34" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="K34" s="11" t="s">
+      <c r="K34" s="9" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A35" s="32" t="s">
+      <c r="A35" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="B35" s="31" t="s">
+      <c r="B35" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="E35" s="23" t="s">
+      <c r="E35" s="21" t="s">
         <v>8</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="G35" s="11" t="s">
+      <c r="G35" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="I35" s="23" t="s">
+      <c r="I35" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="J35" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="K35" s="11" t="s">
+      <c r="J35" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="K35" s="9" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E36" s="28" t="s">
+      <c r="E36" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="F36" s="37" t="s">
+      <c r="F36" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="G36" s="36" t="s">
+      <c r="G36" s="33" t="s">
         <v>126</v>
       </c>
-      <c r="I36" s="22" t="s">
+      <c r="I36" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="J36" s="16" t="s">
+      <c r="J36" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="K36" s="12" t="s">
+      <c r="K36" s="10" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="I37" s="22" t="s">
+      <c r="I37" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="J37" s="16" t="s">
+      <c r="J37" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="K37" s="12" t="s">
+      <c r="K37" s="10" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="I38" s="22" t="s">
+      <c r="I38" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="J38" s="16" t="s">
+      <c r="J38" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="K38" s="11" t="s">
+      <c r="K38" s="9" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="I39" s="28" t="s">
+      <c r="I39" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="J39" s="19" t="s">
+      <c r="J39" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="K39" s="13" t="s">
+      <c r="K39" s="11" t="s">
         <v>110</v>
       </c>
     </row>

</xml_diff>